<commit_message>
time to finish basics..
</commit_message>
<xml_diff>
--- a/app_progress.xlsx
+++ b/app_progress.xlsx
@@ -7,37 +7,106 @@
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Checkliste"/>
+    <sheet r:id="rId1" sheetId="1" name="Design Patterns"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
-  <si>
-    <t>TASK</t>
-  </si>
-  <si>
-    <t>DONE</t>
-  </si>
-  <si>
-    <t>Einkaufsliste erstellen</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="31">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Decorator Pattern</t>
+  </si>
+  <si>
+    <t>Kurzinfo</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>Wäsche waschen</t>
-  </si>
-  <si>
-    <t>Zimmer aufräumen</t>
+    <t>Klassendiagramm</t>
+  </si>
+  <si>
+    <t>Dart Beispiel</t>
   </si>
   <si>
     <t>✅</t>
   </si>
   <si>
-    <t>E-Mails beantworten</t>
+    <t>GUI/Flutter Beispiel</t>
+  </si>
+  <si>
+    <t>Chain of Responsibility Pattern</t>
+  </si>
+  <si>
+    <t>Command Pattern</t>
+  </si>
+  <si>
+    <t>Interpreter Pattern</t>
+  </si>
+  <si>
+    <t>Iterator Pattern</t>
+  </si>
+  <si>
+    <t>Mediator Pattern</t>
+  </si>
+  <si>
+    <t>Memento Pattern</t>
+  </si>
+  <si>
+    <t>Observer Pattern</t>
+  </si>
+  <si>
+    <t>State Pattern</t>
+  </si>
+  <si>
+    <t>Strategy Pattern</t>
+  </si>
+  <si>
+    <t>Template Method Pattern</t>
+  </si>
+  <si>
+    <t>Visitor Pattern</t>
+  </si>
+  <si>
+    <t>Abstract Factory Pattern</t>
+  </si>
+  <si>
+    <t>Builder Pattern</t>
+  </si>
+  <si>
+    <t>Factory Method Pattern</t>
+  </si>
+  <si>
+    <t>Prototype Pattern</t>
+  </si>
+  <si>
+    <t>Singleton Pattern</t>
+  </si>
+  <si>
+    <t>Adapter Pattern</t>
+  </si>
+  <si>
+    <t>Bridge Pattern</t>
+  </si>
+  <si>
+    <t>Composite Pattern</t>
+  </si>
+  <si>
+    <t>Facade Pattern</t>
+  </si>
+  <si>
+    <t>Flyweight Pattern</t>
+  </si>
+  <si>
+    <t>Proxy Pattern</t>
   </si>
 </sst>
 </file>
@@ -404,14 +473,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B138"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="25.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="15.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -423,36 +492,790 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+      <c r="A28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="A29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="A30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+      <c r="A32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+      <c r="A33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="A34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+      <c r="A35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+      <c r="A36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+      <c r="A38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+      <c r="A39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+      <c r="A40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="A41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+      <c r="A42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+      <c r="A44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+      <c r="A45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+      <c r="A46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+      <c r="A47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+      <c r="A48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+      <c r="A50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+      <c r="A51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+      <c r="A52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+      <c r="A53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+      <c r="A54" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+      <c r="A56" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+      <c r="A57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+      <c r="A58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+      <c r="A59" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+      <c r="A60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+      <c r="A62" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+      <c r="A63" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+      <c r="A64" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+      <c r="A65" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+      <c r="A66" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+      <c r="A68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B68" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+      <c r="A69" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+      <c r="A70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+      <c r="A71" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+      <c r="A72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+      <c r="A74" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+      <c r="A75" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+      <c r="A76" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+      <c r="A77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+      <c r="A78" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+      <c r="A80" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+      <c r="A81" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+      <c r="A82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+      <c r="A83" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+      <c r="A84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B84" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+      <c r="A85" s="2"/>
+      <c r="B85" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+      <c r="A86" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+      <c r="A87" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+      <c r="A88" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+      <c r="A89" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+      <c r="A90" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+      <c r="A91" s="2"/>
+      <c r="B91" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+      <c r="A92" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+      <c r="A93" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B93" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+      <c r="A94" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+      <c r="A95" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+      <c r="A96" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+      <c r="A97" s="2"/>
+      <c r="B97" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+      <c r="A98" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B98" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+      <c r="A99" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+      <c r="A100" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+      <c r="A101" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
+      <c r="A102" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+      <c r="A103" s="2"/>
+      <c r="B103" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
+      <c r="A104" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B104" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
+      <c r="A105" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B105" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
+      <c r="A106" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
+      <c r="A107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
+      <c r="A108" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B108" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
+      <c r="A109" s="2"/>
+      <c r="B109" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
+      <c r="A110" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
+      <c r="A111" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
+      <c r="A112" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
+      <c r="A113" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
+      <c r="A114" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B114" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
+      <c r="A116" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B116" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
+      <c r="A117" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B117" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
+      <c r="A118" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
+      <c r="A119" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B119" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
+      <c r="A120" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B120" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
+      <c r="A122" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B122" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
+      <c r="A123" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B123" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
+      <c r="A124" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
+      <c r="A125" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B125" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
+      <c r="A126" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B126" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
+      <c r="A127" s="2"/>
+      <c r="B127" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
+      <c r="A128" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B128" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
+      <c r="A129" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B129" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
+      <c r="A130" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B130" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
+      <c r="A131" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B131" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
+      <c r="A132" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B132" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
+      <c r="A133" s="2"/>
+      <c r="B133" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
+      <c r="A134" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B134" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
+      <c r="A135" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B135" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
+      <c r="A136" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B136" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
+      <c r="A137" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B137" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
+      <c r="A138" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B138" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>